<commit_message>
Fix: Support for two timers in quadrature test.
</commit_message>
<xml_diff>
--- a/Documentation/Musings.xlsx
+++ b/Documentation/Musings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="984" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="5385" tabRatio="984" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="120">
   <si>
     <t>wiel diameter</t>
   </si>
@@ -366,6 +366,21 @@
   </si>
   <si>
     <t>ms/period</t>
+  </si>
+  <si>
+    <t>ticks/s</t>
+  </si>
+  <si>
+    <t>timerclock</t>
+  </si>
+  <si>
+    <t>ovf</t>
+  </si>
+  <si>
+    <t>ticks</t>
+  </si>
+  <si>
+    <t>time ovf</t>
   </si>
 </sst>
 </file>
@@ -2233,15 +2248,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>88</v>
       </c>
@@ -2249,7 +2264,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -2272,7 +2287,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -2292,7 +2307,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2313,7 +2328,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -2327,7 +2342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -2341,7 +2356,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2360,8 +2375,17 @@
       <c r="L8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8">
+        <v>16000000</v>
+      </c>
+      <c r="P8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -2374,8 +2398,14 @@
       <c r="E9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>110</v>
+      </c>
+      <c r="O9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -2391,8 +2421,18 @@
       <c r="J10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10">
+        <f>O8/O9</f>
+        <v>15625</v>
+      </c>
+      <c r="P10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -2412,8 +2452,29 @@
       <c r="L11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11">
+        <v>20000</v>
+      </c>
+      <c r="P11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>119</v>
+      </c>
+      <c r="O12">
+        <f>O11/O10</f>
+        <v>1.28</v>
+      </c>
+      <c r="P12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J13">
         <f>J11/K4</f>
         <v>2</v>
@@ -2422,7 +2483,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J14">
         <f>1/J13</f>
         <v>0.5</v>
@@ -2431,7 +2492,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J15">
         <f>J14*65535</f>
         <v>32767.5</v>
@@ -2440,7 +2501,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J16">
         <f>J15/1000</f>
         <v>32.767499999999998</v>

</xml_diff>